<commit_message>
Exercicio 2 base wine FEITO
</commit_message>
<xml_diff>
--- a/resultados/ResultadosJoao.xlsx
+++ b/resultados/ResultadosJoao.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="20">
   <si>
     <t>Base de dados utilizada para treinamento e testes: iris.csv</t>
   </si>
@@ -74,36 +74,6 @@
   </si>
   <si>
     <t>Base de dados utilizada para treinamento e testes: wine.csv</t>
-  </si>
-  <si>
-    <t>0.6316.</t>
-  </si>
-  <si>
-    <t>0.6667.</t>
-  </si>
-  <si>
-    <t>0.8333.</t>
-  </si>
-  <si>
-    <t>0.6111.</t>
-  </si>
-  <si>
-    <t>0.9444.</t>
-  </si>
-  <si>
-    <t>0.7778.</t>
-  </si>
-  <si>
-    <t>0.8235.</t>
-  </si>
-  <si>
-    <t>0.8125.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Média de acerto: 73.79%</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Desvio padrão: 11.54%</t>
   </si>
   <si>
     <t xml:space="preserve"> - Média de acerto: </t>
@@ -116,7 +86,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +95,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -153,7 +131,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -164,6 +142,7 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,8 +426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -560,7 +539,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B17" s="4">
         <f>AVERAGE(B6:B15)</f>
@@ -569,7 +548,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B18" s="5">
         <f>STDEV(B6:B15)</f>
@@ -828,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -884,90 +863,98 @@
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
-        <v>18</v>
+      <c r="B6">
+        <v>0.76919999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
-        <v>19</v>
+      <c r="B7">
+        <v>0.84619999999999995</v>
       </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" t="s">
-        <v>20</v>
+      <c r="B8">
+        <v>0.61539999999999995</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" t="s">
-        <v>21</v>
+      <c r="B9">
+        <v>0.53849999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" t="s">
-        <v>22</v>
+      <c r="B10">
+        <v>0.53849999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B11" t="s">
-        <v>21</v>
+      <c r="B11">
+        <v>0.46150000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B12" t="s">
-        <v>23</v>
+      <c r="B12">
+        <v>0.46150000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B13" t="s">
-        <v>19</v>
+      <c r="B13">
+        <v>0.92310000000000003</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>10</v>
       </c>
-      <c r="B14" t="s">
-        <v>24</v>
+      <c r="B14">
+        <v>0.84619999999999995</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B15" t="s">
-        <v>25</v>
+      <c r="B15">
+        <v>0.61539999999999995</v>
       </c>
     </row>
     <row r="17" spans="1:14">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>18</v>
+      </c>
+      <c r="B17" s="5">
+        <f>AVERAGE(B6:B15)</f>
+        <v>0.66154999999999997</v>
       </c>
     </row>
     <row r="18" spans="1:14">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>19</v>
+      </c>
+      <c r="B18" s="5">
+        <f>STDEV(B6:B15)</f>
+        <v>0.17087045938045822</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -1024,43 +1011,43 @@
         <v>2</v>
       </c>
       <c r="B23">
-        <v>0.63160000000000005</v>
+        <v>0.75</v>
       </c>
       <c r="C23">
-        <v>0.57889999999999997</v>
+        <v>0.75</v>
       </c>
       <c r="D23">
-        <v>0.57889999999999997</v>
+        <v>0.83330000000000004</v>
       </c>
       <c r="E23">
-        <v>0.57889999999999997</v>
+        <v>0.83330000000000004</v>
       </c>
       <c r="F23">
-        <v>0.57889999999999997</v>
+        <v>0.83330000000000004</v>
       </c>
       <c r="G23">
-        <v>0.63160000000000005</v>
+        <v>0.83330000000000004</v>
       </c>
       <c r="H23">
-        <v>0.63160000000000005</v>
+        <v>0.83330000000000004</v>
       </c>
       <c r="I23">
-        <v>0.63160000000000005</v>
+        <v>0.83330000000000004</v>
       </c>
       <c r="J23">
-        <v>0.63160000000000005</v>
+        <v>0.83330000000000004</v>
       </c>
       <c r="K23">
-        <v>0.63160000000000005</v>
+        <v>0.83330000000000004</v>
       </c>
       <c r="L23">
-        <v>0.63160000000000005</v>
+        <v>0.83330000000000004</v>
       </c>
       <c r="M23">
-        <v>0.63160000000000005</v>
+        <v>0.83330000000000004</v>
       </c>
       <c r="N23">
-        <v>0.63160000000000005</v>
+        <v>0.76919999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -1068,43 +1055,43 @@
         <v>3</v>
       </c>
       <c r="B24">
-        <v>0.72219999999999995</v>
+        <v>0.66669999999999996</v>
       </c>
       <c r="C24">
-        <v>0.55559999999999998</v>
+        <v>0.83330000000000004</v>
       </c>
       <c r="D24">
-        <v>0.55559999999999998</v>
+        <v>0.83330000000000004</v>
       </c>
       <c r="E24">
-        <v>0.66669999999999996</v>
+        <v>0.83330000000000004</v>
       </c>
       <c r="F24">
-        <v>0.66669999999999996</v>
+        <v>0.91669999999999996</v>
       </c>
       <c r="G24">
-        <v>0.66669999999999996</v>
+        <v>0.91669999999999996</v>
       </c>
       <c r="H24">
-        <v>0.66669999999999996</v>
+        <v>0.91669999999999996</v>
       </c>
       <c r="I24">
-        <v>0.66669999999999996</v>
+        <v>0.91669999999999996</v>
       </c>
       <c r="J24">
-        <v>0.66669999999999996</v>
+        <v>0.91669999999999996</v>
       </c>
       <c r="K24">
-        <v>0.66669999999999996</v>
+        <v>0.91669999999999996</v>
       </c>
       <c r="L24">
-        <v>0.66669999999999996</v>
+        <v>0.91669999999999996</v>
       </c>
       <c r="M24">
-        <v>0.66669999999999996</v>
+        <v>0.91669999999999996</v>
       </c>
       <c r="N24">
-        <v>0.66669999999999996</v>
+        <v>0.84619999999999995</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -1112,43 +1099,43 @@
         <v>4</v>
       </c>
       <c r="B25">
-        <v>0.77780000000000005</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="C25">
-        <v>0.77780000000000005</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="D25">
-        <v>0.77780000000000005</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="E25">
-        <v>0.83330000000000004</v>
+        <v>0.66669999999999996</v>
       </c>
       <c r="F25">
-        <v>0.83330000000000004</v>
+        <v>0.66669999999999996</v>
       </c>
       <c r="G25">
-        <v>0.83330000000000004</v>
+        <v>0.66669999999999996</v>
       </c>
       <c r="H25">
-        <v>0.83330000000000004</v>
+        <v>0.66669999999999996</v>
       </c>
       <c r="I25">
-        <v>0.83330000000000004</v>
+        <v>0.66669999999999996</v>
       </c>
       <c r="J25">
-        <v>0.83330000000000004</v>
+        <v>0.66669999999999996</v>
       </c>
       <c r="K25">
-        <v>0.83330000000000004</v>
+        <v>0.66669999999999996</v>
       </c>
       <c r="L25">
-        <v>0.83330000000000004</v>
+        <v>0.66669999999999996</v>
       </c>
       <c r="M25">
-        <v>0.83330000000000004</v>
+        <v>0.66669999999999996</v>
       </c>
       <c r="N25">
-        <v>0.83330000000000004</v>
+        <v>0.61539999999999995</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -1156,43 +1143,43 @@
         <v>5</v>
       </c>
       <c r="B26">
-        <v>0.66669999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="C26">
-        <v>0.66669999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="D26">
-        <v>0.61109999999999998</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="E26">
-        <v>0.55559999999999998</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="F26">
-        <v>0.61109999999999998</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="G26">
-        <v>0.61109999999999998</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="H26">
-        <v>0.61109999999999998</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="I26">
-        <v>0.61109999999999998</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="J26">
-        <v>0.61109999999999998</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="K26">
-        <v>0.61109999999999998</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="L26">
-        <v>0.61109999999999998</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="M26">
-        <v>0.61109999999999998</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="N26">
-        <v>0.61109999999999998</v>
+        <v>0.53849999999999998</v>
       </c>
     </row>
     <row r="27" spans="1:14">
@@ -1200,43 +1187,43 @@
         <v>6</v>
       </c>
       <c r="B27">
-        <v>0.94440000000000002</v>
+        <v>0.75</v>
       </c>
       <c r="C27">
-        <v>0.94440000000000002</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="D27">
-        <v>0.94440000000000002</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="E27">
-        <v>0.94440000000000002</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="F27">
-        <v>0.94440000000000002</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="G27">
-        <v>0.94440000000000002</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="H27">
-        <v>0.94440000000000002</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="I27">
-        <v>0.94440000000000002</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="J27">
-        <v>0.94440000000000002</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="K27">
-        <v>0.94440000000000002</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="L27">
-        <v>0.94440000000000002</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="M27">
-        <v>0.94440000000000002</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="N27">
-        <v>0.94440000000000002</v>
+        <v>0.58330000000000004</v>
       </c>
     </row>
     <row r="28" spans="1:14">
@@ -1244,43 +1231,43 @@
         <v>7</v>
       </c>
       <c r="B28">
-        <v>0.66669999999999996</v>
+        <v>0.75</v>
       </c>
       <c r="C28">
-        <v>0.61109999999999998</v>
+        <v>0.41670000000000001</v>
       </c>
       <c r="D28">
-        <v>0.61109999999999998</v>
+        <v>0.41670000000000001</v>
       </c>
       <c r="E28">
-        <v>0.61109999999999998</v>
+        <v>0.5</v>
       </c>
       <c r="F28">
-        <v>0.61109999999999998</v>
+        <v>0.5</v>
       </c>
       <c r="G28">
-        <v>0.61109999999999998</v>
+        <v>0.5</v>
       </c>
       <c r="H28">
-        <v>0.61109999999999998</v>
+        <v>0.5</v>
       </c>
       <c r="I28">
-        <v>0.61109999999999998</v>
+        <v>0.5</v>
       </c>
       <c r="J28">
-        <v>0.61109999999999998</v>
+        <v>0.5</v>
       </c>
       <c r="K28">
-        <v>0.61109999999999998</v>
+        <v>0.5</v>
       </c>
       <c r="L28">
-        <v>0.61109999999999998</v>
+        <v>0.5</v>
       </c>
       <c r="M28">
-        <v>0.61109999999999998</v>
+        <v>0.5</v>
       </c>
       <c r="N28">
-        <v>0.61109999999999998</v>
+        <v>0.46150000000000002</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -1288,43 +1275,43 @@
         <v>8</v>
       </c>
       <c r="B29">
-        <v>0.66669999999999996</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="C29">
-        <v>0.66669999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="D29">
-        <v>0.66669999999999996</v>
+        <v>0.41670000000000001</v>
       </c>
       <c r="E29">
-        <v>0.77780000000000005</v>
+        <v>0.5</v>
       </c>
       <c r="F29">
-        <v>0.77780000000000005</v>
+        <v>0.5</v>
       </c>
       <c r="G29">
-        <v>0.77780000000000005</v>
+        <v>0.5</v>
       </c>
       <c r="H29">
-        <v>0.77780000000000005</v>
+        <v>0.5</v>
       </c>
       <c r="I29">
-        <v>0.77780000000000005</v>
+        <v>0.5</v>
       </c>
       <c r="J29">
-        <v>0.77780000000000005</v>
+        <v>0.5</v>
       </c>
       <c r="K29">
-        <v>0.77780000000000005</v>
+        <v>0.5</v>
       </c>
       <c r="L29">
-        <v>0.77780000000000005</v>
+        <v>0.5</v>
       </c>
       <c r="M29">
-        <v>0.77780000000000005</v>
+        <v>0.5</v>
       </c>
       <c r="N29">
-        <v>0.77780000000000005</v>
+        <v>0.46150000000000002</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -1332,43 +1319,43 @@
         <v>9</v>
       </c>
       <c r="B30">
-        <v>0.38890000000000002</v>
+        <v>0.75</v>
       </c>
       <c r="C30">
-        <v>0.61109999999999998</v>
+        <v>0.75</v>
       </c>
       <c r="D30">
-        <v>0.61109999999999998</v>
+        <v>0.75</v>
       </c>
       <c r="E30">
-        <v>0.61109999999999998</v>
+        <v>0.91669999999999996</v>
       </c>
       <c r="F30">
-        <v>0.66669999999999996</v>
+        <v>0.91669999999999996</v>
       </c>
       <c r="G30">
-        <v>0.66669999999999996</v>
+        <v>1</v>
       </c>
       <c r="H30">
-        <v>0.66669999999999996</v>
+        <v>1</v>
       </c>
       <c r="I30">
-        <v>0.66669999999999996</v>
+        <v>1</v>
       </c>
       <c r="J30">
-        <v>0.66669999999999996</v>
+        <v>1</v>
       </c>
       <c r="K30">
-        <v>0.66669999999999996</v>
+        <v>1</v>
       </c>
       <c r="L30">
-        <v>0.66669999999999996</v>
+        <v>1</v>
       </c>
       <c r="M30">
-        <v>0.66669999999999996</v>
+        <v>1</v>
       </c>
       <c r="N30">
-        <v>0.66669999999999996</v>
+        <v>0.92310000000000003</v>
       </c>
     </row>
     <row r="31" spans="1:14">
@@ -1376,43 +1363,43 @@
         <v>10</v>
       </c>
       <c r="B31">
-        <v>0.64710000000000001</v>
+        <v>0.83330000000000004</v>
       </c>
       <c r="C31">
-        <v>0.70589999999999997</v>
+        <v>0.91669999999999996</v>
       </c>
       <c r="D31">
-        <v>0.76470000000000005</v>
+        <v>0.91669999999999996</v>
       </c>
       <c r="E31">
-        <v>0.82350000000000001</v>
+        <v>0.91669999999999996</v>
       </c>
       <c r="F31">
-        <v>0.82350000000000001</v>
+        <v>0.91669999999999996</v>
       </c>
       <c r="G31">
-        <v>0.82350000000000001</v>
+        <v>0.91669999999999996</v>
       </c>
       <c r="H31">
-        <v>0.82350000000000001</v>
+        <v>0.91669999999999996</v>
       </c>
       <c r="I31">
-        <v>0.82350000000000001</v>
+        <v>0.91669999999999996</v>
       </c>
       <c r="J31">
-        <v>0.82350000000000001</v>
+        <v>0.91669999999999996</v>
       </c>
       <c r="K31">
-        <v>0.82350000000000001</v>
+        <v>0.91669999999999996</v>
       </c>
       <c r="L31">
-        <v>0.82350000000000001</v>
+        <v>0.91669999999999996</v>
       </c>
       <c r="M31">
-        <v>0.82350000000000001</v>
+        <v>0.91669999999999996</v>
       </c>
       <c r="N31">
-        <v>0.82350000000000001</v>
+        <v>0.84619999999999995</v>
       </c>
     </row>
     <row r="32" spans="1:14">
@@ -1423,128 +1410,157 @@
         <v>0.75</v>
       </c>
       <c r="C32">
-        <v>0.75</v>
+        <v>0.66669999999999996</v>
       </c>
       <c r="D32">
-        <v>0.75</v>
+        <v>0.66669999999999996</v>
       </c>
       <c r="E32">
-        <v>0.8125</v>
+        <v>0.66669999999999996</v>
       </c>
       <c r="F32">
-        <v>0.8125</v>
+        <v>0.66669999999999996</v>
       </c>
       <c r="G32">
-        <v>0.8125</v>
+        <v>0.66669999999999996</v>
       </c>
       <c r="H32">
-        <v>0.8125</v>
+        <v>0.66669999999999996</v>
       </c>
       <c r="I32">
-        <v>0.8125</v>
+        <v>0.66669999999999996</v>
       </c>
       <c r="J32">
-        <v>0.8125</v>
+        <v>0.66669999999999996</v>
       </c>
       <c r="K32">
-        <v>0.8125</v>
+        <v>0.66669999999999996</v>
       </c>
       <c r="L32">
-        <v>0.8125</v>
+        <v>0.66669999999999996</v>
       </c>
       <c r="M32">
-        <v>0.8125</v>
+        <v>0.66669999999999996</v>
       </c>
       <c r="N32">
-        <v>0.8125</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14">
+        <v>0.61539999999999995</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="O33" s="6"/>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" t="s">
         <v>13</v>
       </c>
       <c r="B34" s="1">
-        <v>0.68620000000000003</v>
+        <f>AVERAGE(B23:B32)</f>
+        <v>0.69166000000000005</v>
       </c>
       <c r="C34" s="1">
-        <v>0.68679999999999997</v>
+        <f t="shared" ref="C34:N34" si="0">AVERAGE(C23:C32)</f>
+        <v>0.64999999999999991</v>
       </c>
       <c r="D34" s="1">
-        <v>0.68710000000000004</v>
+        <f t="shared" si="0"/>
+        <v>0.65832999999999997</v>
       </c>
       <c r="E34" s="1">
-        <v>0.72150000000000003</v>
+        <f t="shared" si="0"/>
+        <v>0.7</v>
       </c>
       <c r="F34" s="1">
-        <v>0.73260000000000003</v>
+        <f t="shared" si="0"/>
+        <v>0.70833999999999986</v>
       </c>
       <c r="G34" s="1">
-        <v>0.7379</v>
+        <f t="shared" si="0"/>
+        <v>0.71666999999999992</v>
       </c>
       <c r="H34" s="1">
-        <v>0.7379</v>
+        <f t="shared" si="0"/>
+        <v>0.71666999999999992</v>
       </c>
       <c r="I34" s="1">
-        <v>0.7379</v>
+        <f>AVERAGE(I23:I32)</f>
+        <v>0.71666999999999992</v>
       </c>
       <c r="J34" s="1">
-        <v>0.7379</v>
+        <f t="shared" si="0"/>
+        <v>0.71666999999999992</v>
       </c>
       <c r="K34" s="1">
-        <v>0.7379</v>
+        <f t="shared" si="0"/>
+        <v>0.71666999999999992</v>
       </c>
       <c r="L34" s="1">
-        <v>0.7379</v>
+        <f t="shared" si="0"/>
+        <v>0.71666999999999992</v>
       </c>
       <c r="M34" s="1">
-        <v>0.7379</v>
+        <f t="shared" si="0"/>
+        <v>0.71666999999999992</v>
       </c>
       <c r="N34" s="1">
-        <v>0.7379</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14">
+        <f t="shared" si="0"/>
+        <v>0.6660299999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35" t="s">
         <v>14</v>
       </c>
       <c r="B35" s="1">
-        <v>0.13919999999999999</v>
+        <f>STDEV(B23:B32)</f>
+        <v>0.1043072406137</v>
       </c>
       <c r="C35" s="1">
-        <v>0.11550000000000001</v>
+        <f t="shared" ref="C35:N35" si="1">STDEV(C23:C32)</f>
+        <v>0.16101529948010168</v>
       </c>
       <c r="D35" s="1">
-        <v>0.1207</v>
+        <f t="shared" si="1"/>
+        <v>0.1732423225812138</v>
       </c>
       <c r="E35" s="1">
-        <v>0.13300000000000001</v>
+        <f t="shared" si="1"/>
+        <v>0.16292845055422395</v>
       </c>
       <c r="F35" s="1">
-        <v>0.12180000000000001</v>
+        <f t="shared" si="1"/>
+        <v>0.17237090628448176</v>
       </c>
       <c r="G35" s="1">
-        <v>0.1154</v>
+        <f t="shared" si="1"/>
+        <v>0.18510157601826252</v>
       </c>
       <c r="H35" s="1">
-        <v>0.1154</v>
+        <f t="shared" si="1"/>
+        <v>0.18510157601826252</v>
       </c>
       <c r="I35" s="1">
-        <v>0.1154</v>
+        <f t="shared" si="1"/>
+        <v>0.18510157601826252</v>
       </c>
       <c r="J35" s="1">
-        <v>0.1154</v>
+        <f t="shared" si="1"/>
+        <v>0.18510157601826252</v>
       </c>
       <c r="K35" s="1">
-        <v>0.1154</v>
+        <f t="shared" si="1"/>
+        <v>0.18510157601826252</v>
       </c>
       <c r="L35" s="1">
-        <v>0.1154</v>
+        <f t="shared" si="1"/>
+        <v>0.18510157601826252</v>
       </c>
       <c r="M35" s="1">
-        <v>0.1154</v>
+        <f t="shared" si="1"/>
+        <v>0.18510157601826252</v>
       </c>
       <c r="N35" s="1">
-        <v>0.1154</v>
+        <f t="shared" si="1"/>
+        <v>0.1678463189282918</v>
       </c>
     </row>
   </sheetData>
@@ -1553,5 +1569,6 @@
     <mergeCell ref="A3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>